<commit_message>
update: user.blade->tambah select dept, api->route->get-departemen, getresponse->function->getbagian;
</commit_message>
<xml_diff>
--- a/public/user-import.xlsx
+++ b/public/user-import.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\pengelolaan_aset\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{084B0822-30B1-4FF3-B74E-3081C07D2E2D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A62B120-2CEC-4D5E-A794-D99E40636FCA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1608" yWindow="2172" windowWidth="17280" windowHeight="9072" xr2:uid="{541BC121-9D4A-47F4-B911-DDD22F8B8BE2}"/>
+    <workbookView xWindow="1956" yWindow="2520" windowWidth="17280" windowHeight="9072" xr2:uid="{541BC121-9D4A-47F4-B911-DDD22F8B8BE2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>nama</t>
   </si>
@@ -34,9 +34,6 @@
   </si>
   <si>
     <t>email</t>
-  </si>
-  <si>
-    <t>password</t>
   </si>
   <si>
     <t>role</t>
@@ -395,15 +392,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52E59412-1CF5-427B-BA6E-C6AAFF26B2D6}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -419,9 +416,6 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix(import-user): updated user-import.xlsx template & fix duplicate email when user imported
Took 33 minutes
</commit_message>
<xml_diff>
--- a/public/user-import.xlsx
+++ b/public/user-import.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\pengelolaan_aset\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73E9E61D-0B98-40B1-A52E-FE9F1303884D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{510F9243-77C5-4B34-BC12-8F09A2A0FC95}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{541BC121-9D4A-47F4-B911-DDD22F8B8BE2}"/>
+    <workbookView xWindow="5580" yWindow="16590" windowWidth="21600" windowHeight="11505" xr2:uid="{541BC121-9D4A-47F4-B911-DDD22F8B8BE2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,21 +37,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -75,9 +67,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -392,15 +383,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52E59412-1CF5-427B-BA6E-C6AAFF26B2D6}">
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10:K13"/>
+      <selection activeCell="A2" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -408,13 +399,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="J3" s="1"/>
-      <c r="M3" s="1"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="J10" s="1"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>